<commit_message>
add graphs of performance
</commit_message>
<xml_diff>
--- a/Benchmark AD Tools/benchmark/BenchmarkADTools.xlsx
+++ b/Benchmark AD Tools/benchmark/BenchmarkADTools.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIT CONSULTING\Desktop\TF\Test\Benchmark AD Tools\benchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Desktop\Test\Benchmark AD Tools\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297053B3-8E3D-4E1F-A202-A00BF5FC0ADB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD1D7D7-95BE-4C78-BE78-99623958177B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sumary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>(5*x**2+7*x+2)**2/(x**2+6)</t>
   </si>
@@ -69,37 +69,10 @@
     <t>((6*x**2+x)**2)*((x**5+x**6)**4)</t>
   </si>
   <si>
-    <t>142.56</t>
-  </si>
-  <si>
-    <t>15.5177</t>
-  </si>
-  <si>
-    <t>-30.5888</t>
-  </si>
-  <si>
     <t>-16</t>
   </si>
   <si>
-    <t>1.433</t>
-  </si>
-  <si>
-    <t>1.51424e+06</t>
-  </si>
-  <si>
-    <t>30947.6</t>
-  </si>
-  <si>
-    <t>-3.41446</t>
-  </si>
-  <si>
-    <t>2.5584e+16</t>
-  </si>
-  <si>
     <t>-0.00394458</t>
-  </si>
-  <si>
-    <t>7.61128e+11</t>
   </si>
   <si>
     <t>Function</t>
@@ -133,6 +106,9 @@
   </si>
   <si>
     <t>AD time</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -191,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -202,6 +178,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -218,6 +197,3014 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-419" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Numerical Performance of Automatic Differentiation Tools </a:t>
+            </a:r>
+            <a:endParaRPr lang="es-419" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AlgoPy solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$C$2:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>142.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.51771538367151</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30.588799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4330009728239641</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14130297.444786681</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30947.555555555551</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.51771538367151</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1142691.7510824541</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.414461263533624</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.558399909918854E+16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.9445843308367106E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>761127763968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E3E2-4737-9C6B-13003D502871}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Autograd solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$D$2:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>142.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.51771538367151</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30.588799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4330009728239641</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14130297.444786681</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30947.555555555551</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.51771538367151</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1142691.7510824541</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.414461263533624</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.558399909918854E+16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.9445843308367106E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>761127763968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E3E2-4737-9C6B-13003D502871}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>casADI solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$E$2:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>142.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.5177</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30.588799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>1514240</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>1413030000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30947.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.51771538367151</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1142691.7510824541</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.4144600000000001</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>2.5584E+16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.9445799999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00E+00">
+                  <c:v>761128000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E3E2-4737-9C6B-13003D502871}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Numdifftools solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$F$2:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>142.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.51771538367151</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30.588799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4330009699999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514239.9999999099</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14130297.444788</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30947.55555555</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.51771538</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1142691.7510824299</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.414461263533624</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>2.55839991E+16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00E+00">
+                  <c:v>761127764000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E3E2-4737-9C6B-13003D502871}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AD solution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sumary!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$G$2:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>142.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.51771538367151</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-30.588799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4330009728239641</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14130297.444786681</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30947.555555555551</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.51771538367151</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1142691.7510824541</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.414461263533624</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.558399909918854E+16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.9445843308367106E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>761127763968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E3E2-4737-9C6B-13003D502871}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="316209776"/>
+        <c:axId val="316201248"/>
+        <c:axId val="415624824"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="316209776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316201248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="316201248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316209776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="415624824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="316201248"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-419"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-419" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time Numerical Performance of Automatic Differentiation Tools </a:t>
+            </a:r>
+            <a:endParaRPr lang="es-419" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AlgoPy time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$H$2:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.426935195922852E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5783004760742188E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.33514404296875E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.083135604858398E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9795379638671875E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4450550079345701E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.250028610229492E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0981559753417971E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1702728271484375E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4069080352783201E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.1379203796386719E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.198883056640625E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4939308166503911E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2240409851074221E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3374-41D8-B790-44E4A39C4868}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Autograd time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$I$2:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>5.4907798767089844E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.260208129882812E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0102005004882813E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2401084899902338E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8286705017089841E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8589706420898438E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.919601440429688E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4689903259277338E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6713142395019531E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.08172607421875E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.549720764160156E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0599365234375E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.491806030273438E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2104721069335938E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3374-41D8-B790-44E4A39C4868}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>casADI time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$J$2:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>5.8412551879882813E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6787986755371088E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2714347839355469E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4608116149902338E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7012825012207031E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3691864013671875E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1093101501464844E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.320144653320312E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.660751342773438E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1188468933105469E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3198127746582031E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5892257690429688E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5408477783203125E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2891502380371088E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3374-41D8-B790-44E4A39C4868}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Numdifftools time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$K$2:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2.30259895324707E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2840499877929692E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5010108947753911E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4709701538085942E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2320747375488281E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.486944198608398E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.434015274047852E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4330615997314449E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9860267639160161E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1510124206542969E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8980503082275391E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0020008087158199E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1760463714599609E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1109580993652339E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3374-41D8-B790-44E4A39C4868}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sumary!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AD time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sumary!$L$2:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2.5796890258789063E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.20159912109375E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5091896057128909E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6617774963378909E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.008510589599609E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5902519226074219E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4281272888183591E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.130104064941406E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5088272094726563E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.850128173828125E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8160552978515618E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.7949295043945313E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0909309387207031E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.430511474609375E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3374-41D8-B790-44E4A39C4868}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="417272568"/>
+        <c:axId val="417275192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="417272568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417275192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="417275192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417272568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-419"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="307">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{853AF4F0-EFAD-444A-90E6-FE7207223C2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0988E9BB-F63A-4717-A3FC-C72828236889}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -543,64 +3530,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="B1:G15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -611,8 +3598,8 @@
       <c r="D2" s="3">
         <v>142.56</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
+      <c r="E2" s="3">
+        <v>142.56</v>
       </c>
       <c r="F2" s="3">
         <v>142.56</v>
@@ -636,9 +3623,9 @@
         <v>2.5796890258789063E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -649,8 +3636,8 @@
       <c r="D3" s="3">
         <v>15.51771538367151</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
+      <c r="E3" s="3">
+        <v>15.5177</v>
       </c>
       <c r="F3" s="3">
         <v>15.51771538367151</v>
@@ -674,9 +3661,9 @@
         <v>8.20159912109375E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -687,8 +3674,8 @@
       <c r="D4" s="3">
         <v>-30.588799999999999</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
+      <c r="E4" s="3">
+        <v>-30.588799999999999</v>
       </c>
       <c r="F4" s="3">
         <v>-30.588799999999999</v>
@@ -712,9 +3699,9 @@
         <v>1.5091896057128909E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -726,7 +3713,7 @@
         <v>-16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3">
         <v>-16</v>
@@ -750,9 +3737,9 @@
         <v>1.6617774963378909E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -763,8 +3750,8 @@
       <c r="D6" s="3">
         <v>1.4330009728239641</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
+      <c r="E6" s="3">
+        <v>1.4330000000000001</v>
       </c>
       <c r="F6" s="3">
         <v>1.4330009699999999</v>
@@ -788,9 +3775,9 @@
         <v>1.008510589599609E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -801,8 +3788,8 @@
       <c r="D7" s="3">
         <v>1514240</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
+      <c r="E7" s="4">
+        <v>1514240</v>
       </c>
       <c r="F7" s="3">
         <v>1514239.9999999099</v>
@@ -826,9 +3813,9 @@
         <v>1.5902519226074219E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -864,9 +3851,9 @@
         <v>1.4281272888183591E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -877,8 +3864,8 @@
       <c r="D9" s="3">
         <v>30947.555555555551</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
+      <c r="E9" s="3">
+        <v>30947.599999999999</v>
       </c>
       <c r="F9" s="3">
         <v>30947.55555555</v>
@@ -902,9 +3889,9 @@
         <v>1.130104064941406E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -915,8 +3902,8 @@
       <c r="D10" s="3">
         <v>15.51771538367151</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>14</v>
+      <c r="E10" s="3">
+        <v>15.51771538367151</v>
       </c>
       <c r="F10" s="3">
         <v>15.51771538</v>
@@ -940,9 +3927,9 @@
         <v>6.5088272094726563E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -978,9 +3965,9 @@
         <v>1.850128173828125E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
@@ -991,8 +3978,8 @@
       <c r="D12" s="3">
         <v>-3.414461263533624</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
+      <c r="E12" s="3">
+        <v>-3.4144600000000001</v>
       </c>
       <c r="F12" s="3">
         <v>-3.414461263533624</v>
@@ -1016,9 +4003,9 @@
         <v>4.8160552978515618E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>10</v>
@@ -1029,8 +4016,8 @@
       <c r="D13" s="3">
         <v>2.558399909918854E+16</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>21</v>
+      <c r="E13" s="4">
+        <v>2.5584E+16</v>
       </c>
       <c r="F13" s="4">
         <v>2.55839991E+16</v>
@@ -1054,9 +4041,9 @@
         <v>6.7949295043945313E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>11</v>
@@ -1067,11 +4054,11 @@
       <c r="D14" s="3">
         <v>-3.9445843308367106E-3</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
+      <c r="E14" s="3">
+        <v>-3.9445799999999996E-3</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G14" s="2">
         <v>-3.9445843308367106E-3</v>
@@ -1092,9 +4079,9 @@
         <v>2.0909309387207031E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
@@ -1105,8 +4092,8 @@
       <c r="D15" s="3">
         <v>761127763968</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>23</v>
+      <c r="E15" s="4">
+        <v>761128000000</v>
       </c>
       <c r="F15" s="4">
         <v>761127764000</v>
@@ -1132,6 +4119,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1140,11 +4128,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>